<commit_message>
fix in local search and script to generate .csv with results
</commit_message>
<xml_diff>
--- a/FLP/data/results.xlsx
+++ b/FLP/data/results.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\EV-chargers\FLP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5514D68-00CE-4A36-AC95-9C35255B63E1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB5E32C-E4D3-4B61-87BA-188BD3977426}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{6E6F0A83-42D8-4719-9A92-9BDB3BA8A6F9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{6E6F0A83-42D8-4719-9A92-9BDB3BA8A6F9}"/>
   </bookViews>
   <sheets>
     <sheet name="optimal" sheetId="3" r:id="rId1"/>
     <sheet name="Fwd Greedy" sheetId="1" r:id="rId2"/>
     <sheet name="random LS" sheetId="2" r:id="rId3"/>
     <sheet name="local search" sheetId="4" r:id="rId4"/>
-    <sheet name="bounded LS" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -471,7 +470,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -816,7 +815,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="I2" sqref="I2:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1160,8 +1159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD05FF6-6CEB-44B1-BD6A-9F92B0F58576}">
   <dimension ref="A1:Y47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="X33" sqref="X33"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="X50" sqref="X50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3118,7 +3117,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>50</v>
       </c>
@@ -3134,8 +3133,68 @@
       <c r="E34">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>10951</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>10951</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>10951</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34">
+        <v>10951</v>
+      </c>
+      <c r="M34">
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <v>10951</v>
+      </c>
+      <c r="O34">
+        <v>1</v>
+      </c>
+      <c r="P34">
+        <v>10951</v>
+      </c>
+      <c r="Q34">
+        <v>1</v>
+      </c>
+      <c r="R34">
+        <v>10951</v>
+      </c>
+      <c r="S34">
+        <v>1</v>
+      </c>
+      <c r="T34">
+        <v>10951</v>
+      </c>
+      <c r="U34">
+        <v>1</v>
+      </c>
+      <c r="V34">
+        <v>10951</v>
+      </c>
+      <c r="W34">
+        <v>1</v>
+      </c>
+      <c r="X34">
+        <v>10951</v>
+      </c>
+      <c r="Y34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>50</v>
       </c>
@@ -3151,8 +3210,68 @@
       <c r="E35">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>19637</v>
+      </c>
+      <c r="G35">
+        <v>2</v>
+      </c>
+      <c r="H35">
+        <v>19637</v>
+      </c>
+      <c r="I35">
+        <v>2</v>
+      </c>
+      <c r="J35">
+        <v>19637</v>
+      </c>
+      <c r="K35">
+        <v>2</v>
+      </c>
+      <c r="L35">
+        <v>19637</v>
+      </c>
+      <c r="M35">
+        <v>2</v>
+      </c>
+      <c r="N35">
+        <v>19637</v>
+      </c>
+      <c r="O35">
+        <v>2</v>
+      </c>
+      <c r="P35">
+        <v>19637</v>
+      </c>
+      <c r="Q35">
+        <v>2</v>
+      </c>
+      <c r="R35">
+        <v>19637</v>
+      </c>
+      <c r="S35">
+        <v>2</v>
+      </c>
+      <c r="T35">
+        <v>19637</v>
+      </c>
+      <c r="U35">
+        <v>2</v>
+      </c>
+      <c r="V35">
+        <v>19637</v>
+      </c>
+      <c r="W35">
+        <v>2</v>
+      </c>
+      <c r="X35">
+        <v>19637</v>
+      </c>
+      <c r="Y35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>50</v>
       </c>
@@ -3168,8 +3287,68 @@
       <c r="E36">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>85817</v>
+      </c>
+      <c r="G36">
+        <v>3</v>
+      </c>
+      <c r="H36">
+        <v>85817</v>
+      </c>
+      <c r="I36">
+        <v>3</v>
+      </c>
+      <c r="J36">
+        <v>85817</v>
+      </c>
+      <c r="K36">
+        <v>3</v>
+      </c>
+      <c r="L36">
+        <v>85817</v>
+      </c>
+      <c r="M36">
+        <v>3</v>
+      </c>
+      <c r="N36">
+        <v>85817</v>
+      </c>
+      <c r="O36">
+        <v>3</v>
+      </c>
+      <c r="P36">
+        <v>85817</v>
+      </c>
+      <c r="Q36">
+        <v>3</v>
+      </c>
+      <c r="R36">
+        <v>85817</v>
+      </c>
+      <c r="S36">
+        <v>3</v>
+      </c>
+      <c r="T36">
+        <v>85817</v>
+      </c>
+      <c r="U36">
+        <v>3</v>
+      </c>
+      <c r="V36">
+        <v>85817</v>
+      </c>
+      <c r="W36">
+        <v>3</v>
+      </c>
+      <c r="X36">
+        <v>85817</v>
+      </c>
+      <c r="Y36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>50</v>
       </c>
@@ -3185,8 +3364,68 @@
       <c r="E37">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>239644</v>
+      </c>
+      <c r="G37">
+        <v>6</v>
+      </c>
+      <c r="H37">
+        <v>239644</v>
+      </c>
+      <c r="I37">
+        <v>6</v>
+      </c>
+      <c r="J37">
+        <v>239644</v>
+      </c>
+      <c r="K37">
+        <v>6</v>
+      </c>
+      <c r="L37">
+        <v>239644</v>
+      </c>
+      <c r="M37">
+        <v>6</v>
+      </c>
+      <c r="N37">
+        <v>239644</v>
+      </c>
+      <c r="O37">
+        <v>6</v>
+      </c>
+      <c r="P37">
+        <v>239644</v>
+      </c>
+      <c r="Q37">
+        <v>6</v>
+      </c>
+      <c r="R37">
+        <v>239644</v>
+      </c>
+      <c r="S37">
+        <v>6</v>
+      </c>
+      <c r="T37">
+        <v>239644</v>
+      </c>
+      <c r="U37">
+        <v>6</v>
+      </c>
+      <c r="V37">
+        <v>239644</v>
+      </c>
+      <c r="W37">
+        <v>6</v>
+      </c>
+      <c r="X37">
+        <v>239644</v>
+      </c>
+      <c r="Y37">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>50</v>
       </c>
@@ -3202,8 +3441,68 @@
       <c r="E38">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>704312</v>
+      </c>
+      <c r="G38">
+        <v>15</v>
+      </c>
+      <c r="H38">
+        <v>704312</v>
+      </c>
+      <c r="I38">
+        <v>14</v>
+      </c>
+      <c r="J38">
+        <v>704312</v>
+      </c>
+      <c r="K38">
+        <v>15</v>
+      </c>
+      <c r="L38">
+        <v>704312</v>
+      </c>
+      <c r="M38">
+        <v>15</v>
+      </c>
+      <c r="N38">
+        <v>704312</v>
+      </c>
+      <c r="O38">
+        <v>15</v>
+      </c>
+      <c r="P38">
+        <v>704312</v>
+      </c>
+      <c r="Q38">
+        <v>15</v>
+      </c>
+      <c r="R38">
+        <v>704312</v>
+      </c>
+      <c r="S38">
+        <v>14</v>
+      </c>
+      <c r="T38">
+        <v>704312</v>
+      </c>
+      <c r="U38">
+        <v>14</v>
+      </c>
+      <c r="V38">
+        <v>704312</v>
+      </c>
+      <c r="W38">
+        <v>15</v>
+      </c>
+      <c r="X38">
+        <v>704312</v>
+      </c>
+      <c r="Y38">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>50</v>
       </c>
@@ -3219,8 +3518,68 @@
       <c r="E39">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>1462963</v>
+      </c>
+      <c r="G39">
+        <v>46</v>
+      </c>
+      <c r="H39">
+        <v>1462963</v>
+      </c>
+      <c r="I39">
+        <v>45</v>
+      </c>
+      <c r="J39">
+        <v>1462963</v>
+      </c>
+      <c r="K39">
+        <v>45</v>
+      </c>
+      <c r="L39">
+        <v>1462963</v>
+      </c>
+      <c r="M39">
+        <v>44</v>
+      </c>
+      <c r="N39">
+        <v>1462963</v>
+      </c>
+      <c r="O39">
+        <v>48</v>
+      </c>
+      <c r="P39">
+        <v>1462963</v>
+      </c>
+      <c r="Q39">
+        <v>50</v>
+      </c>
+      <c r="R39">
+        <v>1462963</v>
+      </c>
+      <c r="S39">
+        <v>47</v>
+      </c>
+      <c r="T39">
+        <v>1462963</v>
+      </c>
+      <c r="U39">
+        <v>50</v>
+      </c>
+      <c r="V39">
+        <v>1462963</v>
+      </c>
+      <c r="W39">
+        <v>43</v>
+      </c>
+      <c r="X39">
+        <v>1462963</v>
+      </c>
+      <c r="Y39">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>50</v>
       </c>
@@ -3236,8 +3595,68 @@
       <c r="E42">
         <v>3</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>10951</v>
+      </c>
+      <c r="G42">
+        <v>9</v>
+      </c>
+      <c r="H42">
+        <v>10951</v>
+      </c>
+      <c r="I42">
+        <v>9</v>
+      </c>
+      <c r="J42">
+        <v>10951</v>
+      </c>
+      <c r="K42">
+        <v>9</v>
+      </c>
+      <c r="L42">
+        <v>10951</v>
+      </c>
+      <c r="M42">
+        <v>9</v>
+      </c>
+      <c r="N42">
+        <v>10951</v>
+      </c>
+      <c r="O42">
+        <v>9</v>
+      </c>
+      <c r="P42">
+        <v>10951</v>
+      </c>
+      <c r="Q42">
+        <v>9</v>
+      </c>
+      <c r="R42">
+        <v>10951</v>
+      </c>
+      <c r="S42">
+        <v>9</v>
+      </c>
+      <c r="T42">
+        <v>10951</v>
+      </c>
+      <c r="U42">
+        <v>9</v>
+      </c>
+      <c r="V42">
+        <v>10951</v>
+      </c>
+      <c r="W42">
+        <v>9</v>
+      </c>
+      <c r="X42">
+        <v>10951</v>
+      </c>
+      <c r="Y42">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>50</v>
       </c>
@@ -3253,8 +3672,68 @@
       <c r="E43">
         <v>3</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <v>19252</v>
+      </c>
+      <c r="G43">
+        <v>15</v>
+      </c>
+      <c r="H43">
+        <v>19137</v>
+      </c>
+      <c r="I43">
+        <v>15</v>
+      </c>
+      <c r="J43">
+        <v>19419</v>
+      </c>
+      <c r="K43">
+        <v>15</v>
+      </c>
+      <c r="L43">
+        <v>18825</v>
+      </c>
+      <c r="M43">
+        <v>15</v>
+      </c>
+      <c r="N43">
+        <v>18692</v>
+      </c>
+      <c r="O43">
+        <v>15</v>
+      </c>
+      <c r="P43">
+        <v>19283</v>
+      </c>
+      <c r="Q43">
+        <v>15</v>
+      </c>
+      <c r="R43">
+        <v>19542</v>
+      </c>
+      <c r="S43">
+        <v>15</v>
+      </c>
+      <c r="T43">
+        <v>19491</v>
+      </c>
+      <c r="U43">
+        <v>15</v>
+      </c>
+      <c r="V43">
+        <v>19390</v>
+      </c>
+      <c r="W43">
+        <v>15</v>
+      </c>
+      <c r="X43">
+        <v>19637</v>
+      </c>
+      <c r="Y43">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>50</v>
       </c>
@@ -3270,8 +3749,68 @@
       <c r="E44">
         <v>3</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>85817</v>
+      </c>
+      <c r="G44">
+        <v>28</v>
+      </c>
+      <c r="H44">
+        <v>85817</v>
+      </c>
+      <c r="I44">
+        <v>28</v>
+      </c>
+      <c r="J44">
+        <v>85817</v>
+      </c>
+      <c r="K44">
+        <v>28</v>
+      </c>
+      <c r="L44">
+        <v>85817</v>
+      </c>
+      <c r="M44">
+        <v>28</v>
+      </c>
+      <c r="N44">
+        <v>85817</v>
+      </c>
+      <c r="O44">
+        <v>28</v>
+      </c>
+      <c r="P44">
+        <v>85817</v>
+      </c>
+      <c r="Q44">
+        <v>28</v>
+      </c>
+      <c r="R44">
+        <v>85817</v>
+      </c>
+      <c r="S44">
+        <v>28</v>
+      </c>
+      <c r="T44">
+        <v>85817</v>
+      </c>
+      <c r="U44">
+        <v>28</v>
+      </c>
+      <c r="V44">
+        <v>85817</v>
+      </c>
+      <c r="W44">
+        <v>28</v>
+      </c>
+      <c r="X44">
+        <v>85817</v>
+      </c>
+      <c r="Y44">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>50</v>
       </c>
@@ -3287,8 +3826,68 @@
       <c r="E45">
         <v>3</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <v>239644</v>
+      </c>
+      <c r="G45">
+        <v>53</v>
+      </c>
+      <c r="H45">
+        <v>239644</v>
+      </c>
+      <c r="I45">
+        <v>56</v>
+      </c>
+      <c r="J45">
+        <v>239644</v>
+      </c>
+      <c r="K45">
+        <v>56</v>
+      </c>
+      <c r="L45">
+        <v>239644</v>
+      </c>
+      <c r="M45">
+        <v>56</v>
+      </c>
+      <c r="N45">
+        <v>239644</v>
+      </c>
+      <c r="O45">
+        <v>57</v>
+      </c>
+      <c r="P45">
+        <v>239644</v>
+      </c>
+      <c r="Q45">
+        <v>56</v>
+      </c>
+      <c r="R45">
+        <v>239644</v>
+      </c>
+      <c r="S45">
+        <v>57</v>
+      </c>
+      <c r="T45">
+        <v>239644</v>
+      </c>
+      <c r="U45">
+        <v>56</v>
+      </c>
+      <c r="V45">
+        <v>239644</v>
+      </c>
+      <c r="W45">
+        <v>56</v>
+      </c>
+      <c r="X45">
+        <v>239644</v>
+      </c>
+      <c r="Y45">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>50</v>
       </c>
@@ -3304,8 +3903,68 @@
       <c r="E46">
         <v>3</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <v>704312</v>
+      </c>
+      <c r="G46">
+        <v>159</v>
+      </c>
+      <c r="H46">
+        <v>704312</v>
+      </c>
+      <c r="I46">
+        <v>156</v>
+      </c>
+      <c r="J46">
+        <v>704312</v>
+      </c>
+      <c r="K46">
+        <v>150</v>
+      </c>
+      <c r="L46">
+        <v>704312</v>
+      </c>
+      <c r="M46">
+        <v>150</v>
+      </c>
+      <c r="N46">
+        <v>704312</v>
+      </c>
+      <c r="O46">
+        <v>151</v>
+      </c>
+      <c r="P46">
+        <v>704312</v>
+      </c>
+      <c r="Q46">
+        <v>139</v>
+      </c>
+      <c r="R46">
+        <v>704312</v>
+      </c>
+      <c r="S46">
+        <v>150</v>
+      </c>
+      <c r="T46">
+        <v>704312</v>
+      </c>
+      <c r="U46">
+        <v>149</v>
+      </c>
+      <c r="V46">
+        <v>704312</v>
+      </c>
+      <c r="W46">
+        <v>149</v>
+      </c>
+      <c r="X46">
+        <v>704312</v>
+      </c>
+      <c r="Y46">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>50</v>
       </c>
@@ -3320,6 +3979,66 @@
       </c>
       <c r="E47">
         <v>3</v>
+      </c>
+      <c r="F47">
+        <v>1459952</v>
+      </c>
+      <c r="G47">
+        <v>423</v>
+      </c>
+      <c r="H47">
+        <v>1462963</v>
+      </c>
+      <c r="I47">
+        <v>421</v>
+      </c>
+      <c r="J47">
+        <v>1462963</v>
+      </c>
+      <c r="K47">
+        <v>404</v>
+      </c>
+      <c r="L47">
+        <v>1461617</v>
+      </c>
+      <c r="M47">
+        <v>405</v>
+      </c>
+      <c r="N47">
+        <v>1462963</v>
+      </c>
+      <c r="O47">
+        <v>404</v>
+      </c>
+      <c r="P47">
+        <v>1462963</v>
+      </c>
+      <c r="Q47">
+        <v>440</v>
+      </c>
+      <c r="R47">
+        <v>1461544</v>
+      </c>
+      <c r="S47">
+        <v>405</v>
+      </c>
+      <c r="T47">
+        <v>1462963</v>
+      </c>
+      <c r="U47">
+        <v>422</v>
+      </c>
+      <c r="V47">
+        <v>1462963</v>
+      </c>
+      <c r="W47">
+        <v>413</v>
+      </c>
+      <c r="X47">
+        <v>1462963</v>
+      </c>
+      <c r="Y47">
+        <v>404</v>
       </c>
     </row>
   </sheetData>
@@ -3332,8 +4051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FF35473-9742-4B22-9105-9EEFA5B1D1F2}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3383,7 +4102,7 @@
         <v>10951</v>
       </c>
       <c r="F2">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3400,10 +4119,10 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>19637</v>
+        <v>16426</v>
       </c>
       <c r="F3">
-        <v>5</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3420,10 +4139,10 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>85817</v>
+        <v>76587</v>
       </c>
       <c r="F4">
-        <v>11</v>
+        <v>657</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3440,10 +4159,10 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>239644</v>
+        <v>216426</v>
       </c>
       <c r="F5">
-        <v>24</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3460,10 +4179,10 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>704312</v>
+        <v>652769</v>
       </c>
       <c r="F6">
-        <v>59</v>
+        <v>3492</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3480,10 +4199,10 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <v>1462963</v>
+        <v>1402630</v>
       </c>
       <c r="F7">
-        <v>115</v>
+        <v>5551</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3503,7 +4222,7 @@
         <v>14854</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -3520,10 +4239,10 @@
         <v>1</v>
       </c>
       <c r="E11">
-        <v>22004</v>
+        <v>20530</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -3540,10 +4259,10 @@
         <v>1</v>
       </c>
       <c r="E12">
-        <v>99511</v>
+        <v>89429</v>
       </c>
       <c r="F12">
-        <v>5</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3560,10 +4279,10 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <v>250810</v>
+        <v>234212</v>
       </c>
       <c r="F13">
-        <v>10</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -3580,10 +4299,10 @@
         <v>1</v>
       </c>
       <c r="E14">
-        <v>715844</v>
+        <v>680509</v>
       </c>
       <c r="F14">
-        <v>25</v>
+        <v>851</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -3600,10 +4319,10 @@
         <v>1</v>
       </c>
       <c r="E15">
-        <v>1564542</v>
+        <v>1477243</v>
       </c>
       <c r="F15">
-        <v>49</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -3640,10 +4359,10 @@
         <v>1</v>
       </c>
       <c r="E19">
-        <v>32421</v>
+        <v>30468</v>
       </c>
       <c r="F19">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -3660,10 +4379,10 @@
         <v>1</v>
       </c>
       <c r="E20">
-        <v>91996</v>
+        <v>84363</v>
       </c>
       <c r="F20">
-        <v>3</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -3680,10 +4399,10 @@
         <v>1</v>
       </c>
       <c r="E21">
-        <v>259252</v>
+        <v>245026</v>
       </c>
       <c r="F21">
-        <v>6</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -3700,10 +4419,10 @@
         <v>1</v>
       </c>
       <c r="E22">
-        <v>743189</v>
+        <v>706192</v>
       </c>
       <c r="F22">
-        <v>14</v>
+        <v>427</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -3720,25 +4439,13 @@
         <v>1</v>
       </c>
       <c r="E23">
-        <v>1537159</v>
+        <v>1465038</v>
       </c>
       <c r="F23">
-        <v>28</v>
+        <v>785</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CDFBF50-F5CB-416B-BB19-A3D70E7A2640}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>